<commit_message>
update 2024 students and yin's paper
</commit_message>
<xml_diff>
--- a/myworks.xlsx
+++ b/myworks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CN-HET-Lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53F5829-1388-4BCC-A9FD-F7E6219EC94F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9600A3AE-4906-4513-87E9-0D777A6CFDC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" firstSheet="2" activeTab="7" xr2:uid="{2265AD8E-7C73-9340-9D54-86819D914AEE}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{2265AD8E-7C73-9340-9D54-86819D914AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="发表论文" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="230">
   <si>
     <t>Chen, S., Zhang, Q., Wang, G., Zhu, L., Li, Y., 2018. Investment strategy for underground gas storage facilities based on real option model considering gas market reform in china. Energy Economics 70, 132–142. https://doi.org/10.1016/j.eneco.2017.12.034</t>
   </si>
@@ -1169,6 +1169,14 @@
   </si>
   <si>
     <t>第十届全国大学生能源经济学术创意大赛华北电力大学校赛本科生组二等奖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全国碳捕集、利用与封存（CCUS）技术研讨会优秀论文二等奖</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Yin, T., Chen, S., Wang, G., Tan, Y., Teng, F., Zhang, Q., 2024. Can Subsidy Policies Achieve Fuel Cell Logistics Vehicle (FCLV) Promotion Targets? Evidence from the Beijing-Tianjin-Hebei Fuel Cell Vehicle Demonstration City Cluster in China. Energy 133270. https://doi.org/10.1016/j.energy.2024.133270</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1637,10 +1645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D26B086-2910-434C-AB97-2AC2ABC062E1}">
-  <dimension ref="A1:A39"/>
+  <dimension ref="A1:A40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1171875" defaultRowHeight="15"/>
@@ -1838,6 +1846,11 @@
     <row r="39" spans="1:1">
       <c r="A39" t="s">
         <v>185</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="5" t="s">
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -1877,6 +1890,7 @@
     <hyperlink ref="A36" r:id="rId32" display="https://doi.org/10.1016/j.energy.2024.130830" xr:uid="{1692811C-DDCD-449F-B771-971B059B4DA8}"/>
     <hyperlink ref="A38" r:id="rId33" display="https://doi.org/10.2139/ssrn.4761945" xr:uid="{D8F4F9DD-75F4-4391-8E66-93DF15C7CBFA}"/>
     <hyperlink ref="A39" r:id="rId34" display="https://doi.org/10.2139/ssrn.4671244" xr:uid="{9AA03955-F948-44BC-8084-ADC7599E413C}"/>
+    <hyperlink ref="A40" r:id="rId35" display="https://doi.org/10.1016/j.energy.2024.133270" xr:uid="{283DFC01-4C78-4682-A678-FEEDCD4449CB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1884,10 +1898,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4C14FA6-174E-FB43-BF02-E436B1D6FEA7}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1171875" defaultRowHeight="15"/>
@@ -1962,7 +1976,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" ht="16.149999999999999">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1970,10 +1984,10 @@
         <v>160</v>
       </c>
       <c r="C6" t="s">
-        <v>161</v>
+        <v>228</v>
       </c>
       <c r="D6">
-        <v>2023</v>
+        <v>2024</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1981,13 +1995,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>214</v>
+        <v>160</v>
       </c>
       <c r="C7" t="s">
-        <v>215</v>
+        <v>161</v>
       </c>
       <c r="D7">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1995,12 +2009,26 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>160</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>217</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>2024</v>
       </c>
     </row>
@@ -3651,7 +3679,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A48A253F-20F1-5F40-90A5-ADDA6B988307}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update paper and style
GB/T 7714—2015（顺序编码，双语，姓名不大写，全部作者，姓名不缩写）
</commit_message>
<xml_diff>
--- a/myworks.xlsx
+++ b/myworks.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\CN-HET-Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wangge/Mygithub/CN-HET-Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F4D93C3-00BB-443F-A9BC-D8E3380D4509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531F1297-8712-8448-91F8-D6DB76008966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2265AD8E-7C73-9340-9D54-86819D914AEE}"/>
+    <workbookView xWindow="-5300" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2265AD8E-7C73-9340-9D54-86819D914AEE}"/>
   </bookViews>
   <sheets>
     <sheet name="发表论文" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="指导研究生毕业论文" sheetId="7" r:id="rId9"/>
     <sheet name="研究生获得奖励" sheetId="8" r:id="rId10"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">发表论文!$A$2:$A$82</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,100 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="234">
-  <si>
-    <t>Chen, S., Zhang, Q., Wang, G., Zhu, L., Li, Y., 2018. Investment strategy for underground gas storage facilities based on real option model considering gas market reform in china. Energy Economics 70, 132–142. https://doi.org/10.1016/j.eneco.2017.12.034</t>
-  </si>
-  <si>
-    <t>Li, Y., Li, H., Wang, G., Liu, X., Zhang, Q., 2019a. Study on the optimal deployment for photovoltaic components recycle in china. Energy Procedia 158, 4298–4303. https://doi.org/10.1016/j.egypro.2019.01.794</t>
-  </si>
-  <si>
-    <t>Li, Y., Wang, G., Mclellan, B., Chen, S.-Y., Zhang, Q., 2018a. Study of the impacts of upstream natural gas market reform in china on infrastructure deployment and social welfare using an SVM-based rolling horizon stochastic game analysis. Petroleum Science 15, 898–911. https://doi.org/10.1007/s12182-018-0238-x</t>
-  </si>
-  <si>
-    <t>Li, Y., Wang, G., Shen, B., Zhang, Q., Liu, B., Xu, R., 2021a. Conception and policy implications of photovoltaic modules end-of-life management in China. WIREs Energy and Environment 10, e387. https://doi.org/10.1002/wene.387</t>
-  </si>
-  <si>
-    <t>Li, Y., Zhang, Q., Wang, G., Liu, X., McLellan, B., 2021b. Modeling and Policy Study for Information Asymmetry Problem of Photovoltaic Module Quality in China. Emerging Markets Finance and Trade 57, 653–667. https://doi.org/10.1080/1540496X.2019.1604337</t>
-  </si>
-  <si>
-    <t>Li, Y., Zhang, Q., Wang, G., Liu, X., Mclellan, B., 2019b. Promotion policies for third party financing in photovoltaic poverty alleviation projects considering social reputation. Journal of Cleaner Production 211, 350–359. https://doi.org/10.1016/j.jclepro.2018.11.179</t>
-  </si>
-  <si>
-    <t>Li, Y., Zhang, Q., Wang, G., Lu, X., 2022. Recycling schemes and supporting policies modeling for photovoltaic modules considering heterogeneous risks. Resources, Conservation and Recycling 180, 106165. https://doi.org/10.1016/j.resconrec.2022.106165</t>
-  </si>
-  <si>
-    <t>Li, Y., Zhang, Q., Wang, G., McLellan, B., Liu, X.F., Wang, L., 2018b. A review of photovoltaic poverty alleviation projects in china: current status, challenge and policy recommendations. Renewable and Sustainable Energy Reviews 94, 214–223. https://doi.org/10.1016/j.rser.2018.06.012</t>
-  </si>
-  <si>
-    <t>Su, D., Zhang, Q., Wang, G., Li, H., 2015. Market analysis of natural gas for district heating in china. Energy Procedia, Clean, Efficient and Affordable Energy for a Sustainable Future: The 7th International Conference on Applied Energy (ICAE2015) 75, 2713–2717. https://doi.org/10.1016/j.egypro.2015.07.693</t>
-  </si>
-  <si>
-    <t>Tang, Y., Zhang, Q., Li, Yaoming, Wang, G., Li, Yan, 2018. Recycling mechanisms and policy suggestions for spent electric vehicles’ power battery -a case of beijing. Journal of Cleaner Production 186, 388–406. https://doi.org/10.1016/j.jclepro.2018.03.043</t>
-  </si>
-  <si>
-    <t>Teng, F., Zhang, Q., Wang, G., Liu, J., Li, H., 2021. A comprehensive review of energy blockchain: Application scenarios and development trends. Int J Energy Res er.7109. https://doi.org/10.1002/er.7109</t>
-  </si>
-  <si>
-    <t>Tian, R., Zhang, Q., Wang, G., 2015. Market analysis of natural gas for power generation in china. Energy Procedia, Clean, Efficient and Affordable Energy for a Sustainable Future: The 7th International Conference on Applied Energy (ICAE2015) 75, 2718–2723. https://doi.org/10.1016/j.egypro.2015.07.699</t>
-  </si>
-  <si>
-    <t>Tian, R., Zhang, Q., Wang, G., Li, H., Chen, S., Li, Y., Tian, Y., 2017. Study on the promotion of natural gas-fired electricity with energy market reform in china using a dynamic game-theoretic model. Applied Energy, Clean, Efficient and Affordable Energy for a Sustainable Future 185, Part 2, 1832–1839. https://doi.org/10.1016/j.apenergy.2015.11.079</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Li, H., Li, Y., Chen, S., 2017a. The impact of social network on the adoption of real-time electricity pricing mechanism. Energy Procedia 142, 3154–3159. https://doi.org/10.1016/j.egypro.2017.12.383</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Li, H., McLellan, B.C., Chen, S., Li, Y., Tian, Y., 2017b. Study on the promotion impact of demand response on distributed PV penetration by using non-cooperative game theoretical analysis. Applied Energy 185, 1869–1878. https://doi.org/10.1016/j.apenergy.2016.01.016</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Li, Y., Li, H., 2018. Policy simulation for promoting residential PV considering anecdotal information exchanges based on social network modelling. Applied Energy 223, 1–10. https://doi.org/10.1016/j.apenergy.2018.04.028</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Li, Y., Mclellan, B.C., 2019a. Efficient and equitable allocation of renewable portfolio standards targets among china’s provinces. Energy Policy 125, 170–180. https://doi.org/10.1016/j.enpol.2018.10.044</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Li, Y., Mclellan, B.C., Pan, X., 2019b. Corrective regulations on renewable energy certificates trading: pursuing an equity-efficiency trade-off. Energy Economics 80, 970–982. https://doi.org/10.1016/j.eneco.2019.03.008</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Mclellan, B.C., Li, H., 2016. Multi-region optimal deployment of renewable energy considering different interregional transmission scenarios. Energy, Sustainable Energy and Environmental Protection 2014 108, 108–118. https://doi.org/10.1016/j.energy.2015.08.060</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Su, B., Shen, B., Li, Y., Li, Z., 2021. Coordination of tradable carbon emission permits market and renewable electricity certificates market in China. Energy Economics 93, 105038. https://doi.org/10.1016/j.eneco.2020.105038</t>
-  </si>
-  <si>
-    <t>Wang, G., Zhang, Q., Tian, R., Li, H., 2015. Combined impacts of RTP and FIT on optimal management for a residential micro-grid. Energy Procedia, Clean, Efficient and Affordable Energy for a Sustainable Future: The 7th International Conference on Applied Energy (ICAE2015) 75, 1666–1672. https://doi.org/10.1016/j.egypro.2015.07.410</t>
-  </si>
-  <si>
-    <t>Yan, J., Wang, G., Chen, S., Zhang, H., Qian, J., Mao, Y., 2022. Harnessing freight platforms to promote the penetration of long-haul heavy-duty hydrogen fuel-cell trucks. Energy 254, 124225. https://doi.org/10.1016/j.energy.2022.124225</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Li, Y., Li, H., Wang, G., Chen, S., 2017a. Study on the impacts of the LNG market reform in china using a SVM based rolling horizon stochastic game analysis. Energy Procedia 105, 3850–3855. https://doi.org/10.1016/j.egypro.2017.03.786</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Li, Z., Wang, G., Li, H., 2016. Study on the impacts of natural gas supply cost on gas flow and infrastructure deployment in china. Applied Energy 162, 1385–1398. https://doi.org/10.1016/j.apenergy.2015.06.058</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Liu, J., Yang, K., Liu, B., Wang, G., 2022. Market adoption simulation of electric vehicle based on social network model considering nudge policies. Energy 259, 124984. https://doi.org/10.1016/j.energy.2022.124984</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Wang, G., Li, H., Li, Y., Chen, S., 2017b. Study on the implementation pathways and key impacts of RPS target in china using a dynamic game-theoretical equilibrium power market model. Energy Procedia 105, 3844–3849. https://doi.org/10.1016/j.egypro.2017.03.784</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Wang, G., Li, Y., Li, H., McLellan, B., Chen, S., 2018. Substitution effect of renewable portfolio standards and renewable energy certificate trading for feed-in tariff. Applied Energy 227, 426–435. https://doi.org/10.1016/j.apenergy.2017.07.118</t>
-  </si>
-  <si>
-    <t>Zhu, L., Lu, H., Zhang, Q., Li, H., Pan, X., Wang, G., Li, Y., 2016. Application of crowdfunding on the financing of EV’s charging piles. Energy Procedia, Clean Energy for Clean City: CUE 2016--Applied Energy Symposium and Forum: Low-Carbon Cities and Urban Energy Systems 104, 336–341. https://doi.org/10.1016/j.egypro.2016.12.057</t>
-  </si>
-  <si>
-    <t>刘雪飞, 张奇, 李彦, 余乐安, 王歌, 2020. 普惠金融支持光伏发电发展的空间效应研究. 中国管理科学 1–10.</t>
-  </si>
-  <si>
-    <t>张奇, 李彦, 王歌, 朱丽晶, 胡滢, 王乐, 2019. 基于复杂网络的电动汽车充电桩众筹市场信用风险建模与分析. 中国管理科学 27, 66–74.</t>
-  </si>
-  <si>
-    <t>陈思源, 张奇, 王歌, 李彦, 2016. 基于博弈分析的我国天然气储气库开发策略及运营模式研究. 石油科学通报 175–182.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="235">
   <si>
     <t>papers</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -920,26 +830,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Teng, F., Zhang, Q., Chen, S., Wang, G., Huang, Z., Wang, L., 2024. Comprehensive effects of policy mixes on the diffusion of heavy-duty hydrogen fuel cell electric trucks in China considering technology learning. Energy Policy 185, 113961. https://doi.org/10.1016/j.enpol.2023.113961</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>承担8学时</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>刘玮, 万燕鸣, 陈思源, 刘畅, 刘琦, 张岩, 王歌, 2023. 基于场景模拟的公路货运新能源车成本效益分析研究. 中国环境科学 43, 5624–5632. https://doi.org/10.19674/j.cnki.issn1000-6923.20230808.003</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Gao Z, Zhang Q, Liu B, Liu J, Wang G, Ni R, Yang K,  2024. The driving factors and mitigation strategy of CO2 emissions from China’s passenger vehicle sector towards carbon neutrality. Energy 294:130830. https://doi.org/10.1016/j.energy.2024.130830.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Wang, L., Zhang, Q., Liu, J., Wang, G., 2024. Science mapping the knowledge domain of electrochemical energy storage technology: A bibliometric review. Journal of Energy Storage 77, 109819. https://doi.org/10.1016/j.est.2023.109819</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>基于“车-电”协同的北京市碳中和路径优化与政策创新研究</t>
   </si>
   <si>
@@ -999,17 +893,6 @@
     <t>碳中和关键金属技术-经济-政策决策优化系统软件</t>
   </si>
   <si>
-    <t>王歌, 张奇, 李彦, 余乐安, 2024. 区块链共享模式下的分布式光伏扩散演化模拟. 系统工程学报 39:189–99. https://doi.org/10.13383/j.cnki.jse.2024.02.003.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Liu, J., Zhang, Q., Teng, F., Wang, L., Wang, G., 2024. A New Investment Decision-Making Model of Hydrogen Energy Storage Technology Based on Real-Time Operation Optimization and Learning Effects. Journal of Energy Storage 96, 112745. https://doi.org/10.2139/ssrn.4761945</t>
-  </si>
-  <si>
-    <t>Zhang, Q., Liu, J., Wang, G., Gao, Z., 2024. A New Optimization Model for Carbon Capture Utilization and Storage (Ccus) Layout Based on High-Resolution Geological Variability. Applied Energy. https://doi.org/10.2139/ssrn.4671244</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>油气生产和消费革命战略分析软件平台</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1176,10 +1059,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Yin, T., Chen, S., Wang, G., Tan, Y., Teng, F., Zhang, Q., 2024. Can Subsidy Policies Achieve Fuel Cell Logistics Vehicle (FCLV) Promotion Targets? Evidence from the Beijing-Tianjin-Hebei Fuel Cell Vehicle Demonstration City Cluster in China. Energy 133270. https://doi.org/10.1016/j.energy.2024.133270</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>碳管理学</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -1194,6 +1073,126 @@
   <si>
     <t>中国电力出版社</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>陈思源, 张奇, 王歌, 李彦. 基于博弈分析的我国天然气储气库开发策略及运营模式研究[J]. 石油科学通报, 2016(01): 175-182.</t>
+  </si>
+  <si>
+    <t>刘玮, 万燕鸣, 陈思源, 刘畅, 刘琦, 张岩, 王歌. 基于场景模拟的公路货运新能源车成本效益分析研究[J/OL]. 中国环境科学, 2023, 43(10): 5624-5632. DOI:10.19674/j.cnki.issn1000-6923.20230808.003.</t>
+  </si>
+  <si>
+    <t>刘雪飞, 张奇, 李彦, 余乐安, 王歌. 普惠金融支持光伏发电发展的空间效应研究[J/OL]. 中国管理科学, 2021, 29(8): 24-34. DOI:10.16381/j.cnki.issn1003-207x.2019.2128.</t>
+  </si>
+  <si>
+    <t>王歌, 张奇, 李彦, 余乐安. 区块链共享模式下的分布式光伏扩散演化模拟[J/OL]. 系统工程学报, 2024, 39(2): 189-199. DOI:10.13383/j.cnki.jse.2024.02.003.</t>
+  </si>
+  <si>
+    <t>张奇, 李彦, 王歌, 朱丽晶, 胡滢, 王乐. 基于复杂网络的电动汽车充电桩众筹市场信用风险建模与分析[J]. 中国管理科学, 2019, 27(08): 66-74.</t>
+  </si>
+  <si>
+    <t>Chen Siyuan, Zhang Qi, Wang Ge, Zhu Lijing, Li Yan. Investment strategy for underground gas storage facilities based on real option model considering gas market reform in china[J/OL]. Energy Economics, 2018, 70: 132-142. DOI:10.1016/j.eneco.2017.12.034.</t>
+  </si>
+  <si>
+    <t>Gao Zhihui, Zhang Qi, Liu Boyu, Liu Jiangfeng, Wang Ge, Ni Ruiyan, Yang Kexin. The driving factors and mitigation strategy of CO2 emissions from China’s passenger vehicle sector towards carbon neutrality[J/OL]. Energy, 2024, 294: 130830. DOI:10.1016/j.energy.2024.130830.</t>
+  </si>
+  <si>
+    <t>Li Yan, Li Hailong, Wang Ge, Liu Xuefei, Zhang Qi. Study on the optimal deployment for photovoltaic components recycle in china[J/OL]. Energy Procedia, 2019, 158: 4298-4303. DOI:10.1016/j.egypro.2019.01.794.</t>
+  </si>
+  <si>
+    <t>Li Yan, Wang Ge, Mclellan Benjamin, Chen Si-Yuan, Zhang Qi. Study of the impacts of upstream natural gas market reform in china on infrastructure deployment and social welfare using an SVM-based rolling horizon stochastic game analysis[J/OL]. Petroleum Science, 2018, 15(4): 898-911. DOI:10.1007/s12182-018-0238-x.</t>
+  </si>
+  <si>
+    <t>Li Yan, Wang Ge, Shen Bo, Zhang Qi, Liu Boyu, Xu Ruoxi. Conception and policy implications of photovoltaic modules end-of-life management in China[J/OL]. WIREs Energy and Environment, 2021, 10(1): e387. DOI:https://doi.org/10.1002/wene.387.</t>
+  </si>
+  <si>
+    <t>Li Yan, Zhang Qi, Wang Ge, McLellan Benjamin, Liu Xue Fei, Wang Le. A review of photovoltaic poverty alleviation projects in china: current status, challenge and policy recommendations[J/OL]. Renewable and Sustainable Energy Reviews, 2018, 94: 214-223. DOI:10.1016/j.rser.2018.06.012.</t>
+  </si>
+  <si>
+    <t>Li Yan, Zhang Qi, Wang Ge, Liu Xuefei, Mclellan Benjamin. Promotion policies for third party financing in photovoltaic poverty alleviation projects considering social reputation[J/OL]. Journal of Cleaner Production, 2019, 211: 350-359. DOI:10.1016/j.jclepro.2018.11.179.</t>
+  </si>
+  <si>
+    <t>Li Yan, Zhang Qi, Wang Ge, Liu Xuefei, McLellan Benjamin. Modeling and Policy Study for Information Asymmetry Problem of Photovoltaic Module Quality in China[J/OL]. Emerging Markets Finance and Trade, 2021, 57(3): 653-667. DOI:10.1080/1540496X.2019.1604337.</t>
+  </si>
+  <si>
+    <t>Li Yan, Zhang Qi, Wang Ge, Lu Xi. Recycling schemes and supporting policies modeling for photovoltaic modules considering heterogeneous risks[J/OL]. Resources, Conservation and Recycling, 2022, 180: 106165. DOI:10.1016/j.resconrec.2022.106165.</t>
+  </si>
+  <si>
+    <t>Liu Jiangfeng, Zhang Qi, Teng Fei, Wang Lu, Wang Ge. A New Investment Decision-Making Model of Hydrogen Energy Storage Technology Based on Real-Time Operation Optimization and Learning Effects[J/OL]. Journal of Energy Storage, 2024, 96: 112745. DOI:10.2139/ssrn.4761945.</t>
+  </si>
+  <si>
+    <t>Qian Jiaqi, Wang Ge, Yin Ting, Mao Yuxuan, Chen Siyuan, Li Yan, Liu Jiangfeng, Zhang Qi. Policy implications of electrifying land freight transport towards carbon-neutral in China[J/OL]. Transport Policy, 2025, 160: 116-124. DOI:10.1016/j.tranpol.2024.11.004.</t>
+  </si>
+  <si>
+    <t>Su Difei, Zhang Qi, Wang Ge, Li Hailong. Market analysis of natural gas for district heating in china[J/OL]. Energy Procedia, 2015, 75: 2713-2717. DOI:10.1016/j.egypro.2015.07.693.</t>
+  </si>
+  <si>
+    <t>Tang Yanyan, Zhang Qi, Li Yaoming, Wang Ge, Li Yan. Recycling mechanisms and policy suggestions for spent electric vehicles’ power battery -a case of beijing[J/OL]. Journal of Cleaner Production, 2018, 186: 388-406. DOI:10.1016/j.jclepro.2018.03.043.</t>
+  </si>
+  <si>
+    <t>Teng Fei, Zhang Qi, Chen Siyuan, Wang Ge, Huang Zhenyue, Wang Lu. Comprehensive effects of policy mixes on the diffusion of heavy-duty hydrogen fuel cell electric trucks in China considering technology learning[J/OL]. Energy Policy, 2024, 185: 113961. DOI:10.1016/j.enpol.2023.113961.</t>
+  </si>
+  <si>
+    <t>Teng Fei, Zhang Qi, Wang Ge, Liu Jiangfeng, Li Hailong. A comprehensive review of energy blockchain: Application scenarios and development trends[J/OL]. International Journal of Energy Research, 2021: er.7109. DOI:10.1002/er.7109.</t>
+  </si>
+  <si>
+    <t>Tian Ruijie, Zhang Qi, Wang Ge. Market analysis of natural gas for power generation in china[J/OL]. Energy Procedia, 2015, 75: 2718-2723. DOI:10.1016/j.egypro.2015.07.699.</t>
+  </si>
+  <si>
+    <t>Tian Ruijie, Zhang Qi, Wang Ge, Li Hailong, Chen Siyuan, Li Yan, Tian Yulu. Study on the promotion of natural gas-fired electricity with energy market reform in china using a dynamic game-theoretic model[J/OL]. Applied Energy, 2017, 185, Part 2: 1832-1839. DOI:10.1016/j.apenergy.2015.11.079.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Li Hailong, McLellan Benjamin C., Chen Siyuan, Li Yan, Tian Yulu. Study on the promotion impact of demand response on distributed PV penetration by using non-cooperative game theoretical analysis[J/OL]. Applied Energy, 2017, 185: 1869-1878. DOI:10.1016/j.apenergy.2016.01.016.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Li Hailong, Li Yan, Chen Siyuan. The impact of social network on the adoption of real-time electricity pricing mechanism[J/OL]. Energy Procedia, 2017, 142: 3154-3159. DOI:10.1016/j.egypro.2017.12.383.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Li Yan, Li Hailong. Policy simulation for promoting residential PV considering anecdotal information exchanges based on social network modelling[J/OL]. Applied Energy, 2018, 223: 1-10. DOI:10.1016/j.apenergy.2018.04.028.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Li Yan, Mclellan Benjamin C. Efficient and equitable allocation of renewable portfolio standards targets among china’s provinces[J/OL]. Energy Policy, 2019, 125: 170-180. DOI:10.1016/j.enpol.2018.10.044.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Li Yan, Mclellan Benjamin C., Pan Xunzhang. Corrective regulations on renewable energy certificates trading: pursuing an equity-efficiency trade-off[J/OL]. Energy Economics, 2019, 80: 970-982. DOI:10.1016/j.eneco.2019.03.008.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Mclellan Benjamin C., Li Hailong. Multi-region optimal deployment of renewable energy considering different interregional transmission scenarios[J/OL]. Energy, 2016, 108: 108-118. DOI:10.1016/j.energy.2015.08.060.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Su Bin, Shen Bo, Li Yan, Li Zhengjun. Coordination of tradable carbon emission permits market and renewable electricity certificates market in China[J/OL]. Energy Economics, 2021, 93: 105038. DOI:10.1016/j.eneco.2020.105038.</t>
+  </si>
+  <si>
+    <t>Wang Ge, Zhang Qi, Tian Ruijie, Li Hailong. Combined impacts of RTP and FIT on optimal management for a residential micro-grid[J/OL]. Energy Procedia, 2015, 75: 1666-1672. DOI:10.1016/j.egypro.2015.07.410.</t>
+  </si>
+  <si>
+    <t>Wang Lu, Zhang Qi, Liu Jiangfeng, Wang Ge. Science mapping the knowledge domain of electrochemical energy storage technology: A bibliometric review[J/OL]. Journal of Energy Storage, 2024, 77: 109819. DOI:10.1016/j.est.2023.109819.</t>
+  </si>
+  <si>
+    <t>Yan Jiaze, Wang Ge, Chen Siyuan, Zhang He, Qian Jiaqi, Mao Yuxuan. Harnessing freight platforms to promote the penetration of long-haul heavy-duty hydrogen fuel-cell trucks[J/OL]. Energy, 2022, 254: 124225. DOI:10.1016/j.energy.2022.124225.</t>
+  </si>
+  <si>
+    <t>Yin Ting, Chen Siyuan, Wang Ge, Tan Yuxuan, Teng Fei, Zhang Qi. Can Subsidy Policies Achieve Fuel Cell Logistics Vehicle (FCLV) Promotion Targets? Evidence from the Beijing-Tianjin-Hebei Fuel Cell Vehicle Demonstration City Cluster in China[J/OL]. Energy, 2024: 133270. DOI:10.1016/j.energy.2024.133270.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Li Yan, Li Hailong, Wang Ge, Chen Siyuan. Study on the impacts of the LNG market reform in china using a SVM based rolling horizon stochastic game analysis[J/OL]. Energy Procedia, 2017, 105: 3850-3855. DOI:10.1016/j.egypro.2017.03.786.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Li Zhan, Wang Ge, Li Hailong. Study on the impacts of natural gas supply cost on gas flow and infrastructure deployment in china[J/OL]. Applied Energy, 2016, 162: 1385-1398. DOI:10.1016/j.apenergy.2015.06.058.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Liu Jiangfeng, Wang Ge, Gao Zhihui. A new optimization model for carbon capture utilization and storage (CCUS) layout based on high-resolution geological variability[J/OL]. Applied Energy, 2024, 363: 123065. DOI:10.1016/j.apenergy.2024.123065.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Liu Jiangfeng, Yang Kexin, Liu Boyu, Wang Ge. Market adoption simulation of electric vehicle based on social network model considering nudge policies[J/OL]. Energy, 2022, 259: 124984. DOI:10.1016/j.energy.2022.124984.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Wang Ge, Li Hailong, Li Yan, Chen Siyuan. Study on the implementation pathways and key impacts of RPS target in china using a dynamic game-theoretical equilibrium power market model[J/OL]. Energy Procedia, 2017, 105: 3844-3849. DOI:10.1016/j.egypro.2017.03.784.</t>
+  </si>
+  <si>
+    <t>Zhang Qi, Wang Ge, Li Yan, Li Hailong, McLellan Benjamin, Chen Siyuan. Substitution effect of renewable portfolio standards and renewable energy certificate trading for feed-in tariff[J/OL]. Applied Energy, 2018, 227: 426-435. DOI:10.1016/j.apenergy.2017.07.118.</t>
+  </si>
+  <si>
+    <t>Zhu Lijing, Lu Huihui, Zhang Qi, Li Hailong, Pan Xunzhang, Wang Ge, Li Yan. Application of crowdfunding on the financing of EV’s charging piles[J/OL]. Energy Procedia, 2016, 104: 336-341. DOI:10.1016/j.egypro.2016.12.057.</t>
   </si>
 </sst>
 </file>
@@ -1334,9 +1333,6 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -1344,6 +1340,9 @@
       <alignment horizontal="left" vertical="center" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1365,9 +1364,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 主题">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1405,7 +1404,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1511,7 +1510,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1653,7 +1652,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1661,252 +1660,263 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D26B086-2910-434C-AB97-2AC2ABC062E1}">
-  <dimension ref="A1:A40"/>
+  <dimension ref="A1:A41"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="5" t="s">
-        <v>0</v>
+      <c r="A2" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
+      <c r="A3" s="8" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:1">
-      <c r="A4" s="5" t="s">
-        <v>2</v>
+      <c r="A4" s="8" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:1">
-      <c r="A5" s="5" t="s">
-        <v>3</v>
+      <c r="A5" s="8" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="6" spans="1:1">
-      <c r="A6" s="5" t="s">
-        <v>4</v>
+      <c r="A6" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="5" t="s">
-        <v>5</v>
+      <c r="A7" s="8" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="5" t="s">
-        <v>6</v>
+      <c r="A8" s="8" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:1">
-      <c r="A9" s="5" t="s">
-        <v>7</v>
+      <c r="A9" s="8" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="5" t="s">
-        <v>8</v>
+      <c r="A10" s="8" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="5" t="s">
-        <v>9</v>
+      <c r="A11" s="8" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="5" t="s">
-        <v>10</v>
+      <c r="A12" s="8" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:1">
-      <c r="A13" s="5" t="s">
-        <v>11</v>
+      <c r="A13" s="8" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="5" t="s">
-        <v>12</v>
+      <c r="A14" s="8" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="15" spans="1:1">
-      <c r="A15" s="5" t="s">
-        <v>13</v>
+      <c r="A15" s="8" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:1">
-      <c r="A16" s="5" t="s">
-        <v>14</v>
+      <c r="A16" s="8" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5" t="s">
-        <v>15</v>
+      <c r="A17" s="8" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:1">
-      <c r="A18" s="5" t="s">
-        <v>16</v>
+      <c r="A18" s="8" t="s">
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:1">
-      <c r="A19" s="5" t="s">
-        <v>17</v>
+      <c r="A19" s="8" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="5" t="s">
-        <v>18</v>
+      <c r="A20" s="8" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="21" spans="1:1">
-      <c r="A21" s="5" t="s">
-        <v>19</v>
+      <c r="A21" s="8" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="5" t="s">
-        <v>20</v>
+      <c r="A22" s="8" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="5" t="s">
-        <v>21</v>
+      <c r="A23" s="8" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="5" t="s">
-        <v>22</v>
+      <c r="A24" s="8" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="5" t="s">
-        <v>23</v>
+      <c r="A25" s="8" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="26" spans="1:1">
-      <c r="A26" s="5" t="s">
-        <v>24</v>
+      <c r="A26" s="8" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="27" spans="1:1">
-      <c r="A27" s="5" t="s">
-        <v>25</v>
+      <c r="A27" s="8" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="5" t="s">
-        <v>26</v>
+      <c r="A28" s="8" t="s">
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="5" t="s">
-        <v>27</v>
+      <c r="A29" s="8" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>28</v>
+      <c r="A30" s="8" t="s">
+        <v>211</v>
       </c>
     </row>
     <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>29</v>
+      <c r="A31" s="8" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>30</v>
+      <c r="A32" s="8" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="5" t="s">
-        <v>162</v>
+      <c r="A33" s="8" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="34" spans="1:1">
-      <c r="A34" s="5" t="s">
-        <v>164</v>
+      <c r="A34" s="8" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:1">
-      <c r="A35" s="5" t="s">
-        <v>166</v>
+      <c r="A35" s="8" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="5" t="s">
-        <v>165</v>
+      <c r="A36" s="8" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>183</v>
+      <c r="A37" s="8" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>184</v>
+      <c r="A38" s="8" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>185</v>
+      <c r="A39" s="8" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="5" t="s">
-        <v>229</v>
+      <c r="A40" s="8" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="8" t="s">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A81">
+    <sortCondition descending="1" ref="A2:A81"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://doi.org/10.1016/j.eneco.2017.12.034" xr:uid="{0AD98BA2-42BF-9B4C-AD98-D765DB4C18CC}"/>
-    <hyperlink ref="A3" r:id="rId2" display="https://doi.org/10.1016/j.egypro.2019.01.794" xr:uid="{5358BF61-D809-D44B-89CE-FAD254281DCA}"/>
-    <hyperlink ref="A4" r:id="rId3" display="https://doi.org/10.1007/s12182-018-0238-x" xr:uid="{EAB2E539-07D9-0642-821C-22761B69691D}"/>
-    <hyperlink ref="A5" r:id="rId4" display="https://doi.org/10.1002/wene.387" xr:uid="{108D4E1A-6A88-6E4A-9530-AE786A9D94A0}"/>
-    <hyperlink ref="A6" r:id="rId5" display="https://doi.org/10.1080/1540496X.2019.1604337" xr:uid="{B1B65355-AB7B-4341-B2C3-8B76C5DDCC90}"/>
-    <hyperlink ref="A7" r:id="rId6" display="https://doi.org/10.1016/j.jclepro.2018.11.179" xr:uid="{EDDAAE44-36E2-684E-A93D-407D401257F8}"/>
-    <hyperlink ref="A8" r:id="rId7" display="https://doi.org/10.1016/j.resconrec.2022.106165" xr:uid="{04191113-07B1-AD48-8B21-81BA2E8BC88A}"/>
-    <hyperlink ref="A9" r:id="rId8" display="https://doi.org/10.1016/j.rser.2018.06.012" xr:uid="{A7AE0646-2390-B84E-A095-C4B4EB8A4CDB}"/>
-    <hyperlink ref="A10" r:id="rId9" display="https://doi.org/10.1016/j.egypro.2015.07.693" xr:uid="{5463A9BE-B366-574D-A28B-F9D1B5915615}"/>
-    <hyperlink ref="A11" r:id="rId10" display="https://doi.org/10.1016/j.jclepro.2018.03.043" xr:uid="{BE1B15E7-3C0D-E944-964F-A1C70D4116A8}"/>
-    <hyperlink ref="A12" r:id="rId11" display="https://doi.org/10.1002/er.7109" xr:uid="{7D819EC7-7F77-7649-83E6-19ABCADBDD87}"/>
-    <hyperlink ref="A13" r:id="rId12" display="https://doi.org/10.1016/j.egypro.2015.07.699" xr:uid="{39DD0553-34B6-0842-8E8F-6EE6F88C1578}"/>
-    <hyperlink ref="A14" r:id="rId13" display="https://doi.org/10.1016/j.apenergy.2015.11.079" xr:uid="{D4E35FF5-1493-CD40-924F-396E9EC13D51}"/>
-    <hyperlink ref="A15" r:id="rId14" display="https://doi.org/10.1016/j.egypro.2017.12.383" xr:uid="{3A7D1CA1-E05B-9C48-99AB-EEEAC4195E96}"/>
-    <hyperlink ref="A16" r:id="rId15" display="https://doi.org/10.1016/j.apenergy.2016.01.016" xr:uid="{35E729BA-CB46-DA49-8061-438DDECE546D}"/>
-    <hyperlink ref="A17" r:id="rId16" display="https://doi.org/10.1016/j.apenergy.2018.04.028" xr:uid="{691553EF-9EDE-8247-8DBC-1D36448A8027}"/>
-    <hyperlink ref="A18" r:id="rId17" display="https://doi.org/10.1016/j.enpol.2018.10.044" xr:uid="{8F01B7E2-1B45-9C4A-9ECC-FD0767D33BAA}"/>
-    <hyperlink ref="A19" r:id="rId18" display="https://doi.org/10.1016/j.eneco.2019.03.008" xr:uid="{CDFF7970-2D39-F141-B070-49D219551906}"/>
-    <hyperlink ref="A20" r:id="rId19" display="https://doi.org/10.1016/j.energy.2015.08.060" xr:uid="{1920461B-775A-8C41-85CF-D637CD57F9DD}"/>
-    <hyperlink ref="A21" r:id="rId20" display="https://doi.org/10.1016/j.eneco.2020.105038" xr:uid="{896163B8-29BB-1146-83B0-B6F9A0B6F882}"/>
-    <hyperlink ref="A22" r:id="rId21" display="https://doi.org/10.1016/j.egypro.2015.07.410" xr:uid="{A6F605EA-0ADA-5446-94C9-F0A3E5C0E082}"/>
-    <hyperlink ref="A23" r:id="rId22" display="https://doi.org/10.1016/j.energy.2022.124225" xr:uid="{BF520865-A496-4E4F-B8AB-C3692EE77C28}"/>
-    <hyperlink ref="A24" r:id="rId23" display="https://doi.org/10.1016/j.egypro.2017.03.786" xr:uid="{F4B0A055-8752-8040-9D20-6BF43B792BB2}"/>
-    <hyperlink ref="A25" r:id="rId24" display="https://doi.org/10.1016/j.apenergy.2015.06.058" xr:uid="{DAE897A2-8CBA-B042-B9EF-75A2C4EDA64E}"/>
-    <hyperlink ref="A26" r:id="rId25" display="https://doi.org/10.1016/j.energy.2022.124984" xr:uid="{2518DE09-060F-A148-8F26-8EF931C86B88}"/>
-    <hyperlink ref="A27" r:id="rId26" display="https://doi.org/10.1016/j.egypro.2017.03.784" xr:uid="{FD7C42F1-BE4C-674E-BEC5-63947A06160C}"/>
-    <hyperlink ref="A28" r:id="rId27" display="https://doi.org/10.1016/j.apenergy.2017.07.118" xr:uid="{4CCB93C4-FDB0-A24E-8BCC-662522AB0151}"/>
-    <hyperlink ref="A29" r:id="rId28" display="https://doi.org/10.1016/j.egypro.2016.12.057" xr:uid="{94EB7264-AD46-7048-A51D-A53AB4AA52E8}"/>
-    <hyperlink ref="A33" r:id="rId29" display="https://doi.org/10.1016/j.enpol.2023.113961" xr:uid="{E3FF8D0C-C845-416E-9BBF-89191686E2DB}"/>
-    <hyperlink ref="A34" r:id="rId30" display="https://doi.org/10.19674/j.cnki.issn1000-6923.20230808.003" xr:uid="{963064A2-B7EC-464F-9EE8-56D41B392947}"/>
-    <hyperlink ref="A35" r:id="rId31" display="https://doi.org/10.1016/j.est.2023.109819" xr:uid="{1AFCA61F-8FC0-46A9-A34E-15E08796E503}"/>
-    <hyperlink ref="A36" r:id="rId32" display="https://doi.org/10.1016/j.energy.2024.130830" xr:uid="{1692811C-DDCD-449F-B771-971B059B4DA8}"/>
-    <hyperlink ref="A38" r:id="rId33" display="https://doi.org/10.2139/ssrn.4761945" xr:uid="{D8F4F9DD-75F4-4391-8E66-93DF15C7CBFA}"/>
-    <hyperlink ref="A39" r:id="rId34" display="https://doi.org/10.2139/ssrn.4671244" xr:uid="{9AA03955-F948-44BC-8084-ADC7599E413C}"/>
-    <hyperlink ref="A40" r:id="rId35" display="https://doi.org/10.1016/j.energy.2024.133270" xr:uid="{283DFC01-4C78-4682-A678-FEEDCD4449CB}"/>
+    <hyperlink ref="A5" r:id="rId1" display="https://doi.org/10.19674/j.cnki.issn1000-6923.20230808.003" xr:uid="{E6F5D7C3-AD73-084C-A11E-89FFB859914E}"/>
+    <hyperlink ref="A4" r:id="rId2" display="https://doi.org/10.16381/j.cnki.issn1003-207x.2019.2128" xr:uid="{F1FEB1D2-F59A-BC4B-8526-F5EA31C92011}"/>
+    <hyperlink ref="A3" r:id="rId3" display="https://doi.org/10.13383/j.cnki.jse.2024.02.003" xr:uid="{1A3C937D-5BA3-774C-8B9C-1D62952E3406}"/>
+    <hyperlink ref="A41" r:id="rId4" display="https://doi.org/10.1016/j.eneco.2017.12.034" xr:uid="{D37EE526-EFA4-2940-A8A9-1A8554388FA0}"/>
+    <hyperlink ref="A40" r:id="rId5" display="https://doi.org/10.1016/j.energy.2024.130830" xr:uid="{F7E39713-D7C9-B348-8E4F-B67F9659F86D}"/>
+    <hyperlink ref="A39" r:id="rId6" display="https://doi.org/10.1016/j.egypro.2019.01.794" xr:uid="{1FE0767D-7EBF-BB4E-84F4-A4E133E10E83}"/>
+    <hyperlink ref="A38" r:id="rId7" display="https://doi.org/10.1007/s12182-018-0238-x" xr:uid="{13BBE4D4-11A0-F84A-A940-811559DE87FC}"/>
+    <hyperlink ref="A37" r:id="rId8" display="https://doi.org/10.1002/wene.387" xr:uid="{D51EF494-A5AE-E248-8C97-54DE4C3E8653}"/>
+    <hyperlink ref="A33" r:id="rId9" display="https://doi.org/10.1016/j.rser.2018.06.012" xr:uid="{8A986EFB-DC14-C640-B0B1-956360F647BA}"/>
+    <hyperlink ref="A35" r:id="rId10" display="https://doi.org/10.1016/j.jclepro.2018.11.179" xr:uid="{9EFC670C-51F4-5E43-836F-87C81135239E}"/>
+    <hyperlink ref="A36" r:id="rId11" display="https://doi.org/10.1080/1540496X.2019.1604337" xr:uid="{8CEC154A-1F28-F44A-BCA7-E362C11FF31A}"/>
+    <hyperlink ref="A34" r:id="rId12" display="https://doi.org/10.1016/j.resconrec.2022.106165" xr:uid="{02EAFF08-B812-A941-BCEC-5A4000497D40}"/>
+    <hyperlink ref="A32" r:id="rId13" display="https://doi.org/10.2139/ssrn.4761945" xr:uid="{76359DB5-208F-3C44-A3B9-9C3BEAF27B1C}"/>
+    <hyperlink ref="A31" r:id="rId14" display="https://doi.org/10.1016/j.tranpol.2024.11.004" xr:uid="{50218D27-4D23-B74A-BC9B-9DF02D2BB1CD}"/>
+    <hyperlink ref="A30" r:id="rId15" display="https://doi.org/10.1016/j.egypro.2015.07.693" xr:uid="{201B86B5-E187-654A-BA40-D80CF97621BD}"/>
+    <hyperlink ref="A29" r:id="rId16" display="https://doi.org/10.1016/j.jclepro.2018.03.043" xr:uid="{C3CAEC7A-E3BF-D746-8D26-2219254523DE}"/>
+    <hyperlink ref="A28" r:id="rId17" display="https://doi.org/10.1016/j.enpol.2023.113961" xr:uid="{109AA462-DCA1-824B-B389-153FC46E0D78}"/>
+    <hyperlink ref="A27" r:id="rId18" display="https://doi.org/10.1002/er.7109" xr:uid="{DFF70265-AF6F-0742-8229-551071C6B600}"/>
+    <hyperlink ref="A25" r:id="rId19" display="https://doi.org/10.1016/j.egypro.2015.07.699" xr:uid="{CC55E01C-0770-E644-AE01-B1C87081A3F2}"/>
+    <hyperlink ref="A26" r:id="rId20" display="https://doi.org/10.1016/j.apenergy.2015.11.079" xr:uid="{81F1092F-9250-A542-8BDB-BBD51C1F1160}"/>
+    <hyperlink ref="A23" r:id="rId21" display="https://doi.org/10.1016/j.apenergy.2016.01.016" xr:uid="{06B94FC3-F022-1D43-A33C-11966CF05BDF}"/>
+    <hyperlink ref="A24" r:id="rId22" display="https://doi.org/10.1016/j.egypro.2017.12.383" xr:uid="{AFC1E29B-1F8C-4347-9732-8B65A9BAB848}"/>
+    <hyperlink ref="A22" r:id="rId23" display="https://doi.org/10.1016/j.apenergy.2018.04.028" xr:uid="{25730D09-2888-544F-A3B5-2C52AA662C2B}"/>
+    <hyperlink ref="A21" r:id="rId24" display="https://doi.org/10.1016/j.enpol.2018.10.044" xr:uid="{08E2A237-DF83-5142-8A0B-292A93A4B9CF}"/>
+    <hyperlink ref="A20" r:id="rId25" display="https://doi.org/10.1016/j.eneco.2019.03.008" xr:uid="{CF028DFD-2CAE-144F-B8F2-6E25A18F65FE}"/>
+    <hyperlink ref="A19" r:id="rId26" display="https://doi.org/10.1016/j.energy.2015.08.060" xr:uid="{B2CBAFA1-002D-E544-BFB2-6ED53D88038D}"/>
+    <hyperlink ref="A18" r:id="rId27" display="https://doi.org/10.1016/j.eneco.2020.105038" xr:uid="{1ACFE16B-FDCB-7542-AC32-FFD1C44B3105}"/>
+    <hyperlink ref="A17" r:id="rId28" display="https://doi.org/10.1016/j.egypro.2015.07.410" xr:uid="{07583A04-4DD2-8B4C-A55C-A2904BD5D44D}"/>
+    <hyperlink ref="A16" r:id="rId29" display="https://doi.org/10.1016/j.est.2023.109819" xr:uid="{9285C00D-8657-9946-A3EC-940D6D13C82B}"/>
+    <hyperlink ref="A15" r:id="rId30" display="https://doi.org/10.1016/j.energy.2022.124225" xr:uid="{6572EA05-680B-E64B-AC1E-806D1A2872CD}"/>
+    <hyperlink ref="A14" r:id="rId31" display="https://doi.org/10.1016/j.energy.2024.133270" xr:uid="{A7891C99-97C3-B14D-9EDE-AAC9A8898F15}"/>
+    <hyperlink ref="A13" r:id="rId32" display="https://doi.org/10.1016/j.egypro.2017.03.786" xr:uid="{74945587-1292-5044-AC85-B11D9A133EE5}"/>
+    <hyperlink ref="A12" r:id="rId33" display="https://doi.org/10.1016/j.apenergy.2015.06.058" xr:uid="{0013A21F-C6A1-9C4F-8DCD-AFF67E057617}"/>
+    <hyperlink ref="A11" r:id="rId34" display="https://doi.org/10.1016/j.apenergy.2024.123065" xr:uid="{C444A3A6-BFBB-6043-8111-467979FD8B85}"/>
+    <hyperlink ref="A10" r:id="rId35" display="https://doi.org/10.1016/j.energy.2022.124984" xr:uid="{840132B1-4DE6-BC41-9FA6-00E5CCF0DC69}"/>
+    <hyperlink ref="A9" r:id="rId36" display="https://doi.org/10.1016/j.egypro.2017.03.784" xr:uid="{D753D908-32D2-7E49-A534-15401F2BB4F2}"/>
+    <hyperlink ref="A8" r:id="rId37" display="https://doi.org/10.1016/j.apenergy.2017.07.118" xr:uid="{661092D1-CF00-CD4A-99E7-AD0C07DA78FF}"/>
+    <hyperlink ref="A7" r:id="rId38" display="https://doi.org/10.1016/j.egypro.2016.12.057" xr:uid="{90B8C809-78BA-7643-BBF7-7B2B000B6ACB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1920,20 +1930,20 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1941,10 +1951,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="D2">
         <v>2023</v>
@@ -1955,38 +1965,38 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>203</v>
+        <v>165</v>
       </c>
       <c r="C3" t="s">
-        <v>154</v>
+        <v>123</v>
       </c>
       <c r="D3">
         <v>2023</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25">
+    <row r="4" spans="1:4" ht="18">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="D4">
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25">
+    <row r="5" spans="1:4" ht="18">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>157</v>
+        <v>126</v>
       </c>
       <c r="D5">
         <v>2023</v>
@@ -1997,10 +2007,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C6" t="s">
-        <v>228</v>
+        <v>190</v>
       </c>
       <c r="D6">
         <v>2024</v>
@@ -2011,10 +2021,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C7" t="s">
-        <v>161</v>
+        <v>130</v>
       </c>
       <c r="D7">
         <v>2023</v>
@@ -2025,10 +2035,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>214</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
-        <v>215</v>
+        <v>177</v>
       </c>
       <c r="D8">
         <v>2024</v>
@@ -2039,10 +2049,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>160</v>
+        <v>129</v>
       </c>
       <c r="C9" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="D9">
         <v>2024</v>
@@ -2059,70 +2069,70 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82FFF91B-78E0-4A8D-AC15-0F3D3EB2758B}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="16.5">
-      <c r="A1" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>205</v>
+    <row r="1" spans="1:6" ht="17">
+      <c r="A1" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>167</v>
       </c>
       <c r="C1" t="s">
-        <v>207</v>
+        <v>169</v>
       </c>
       <c r="D1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="E1" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="F1" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>216</v>
+        <v>178</v>
       </c>
       <c r="B2" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="D2">
         <v>2024</v>
       </c>
       <c r="E2" t="s">
-        <v>210</v>
+        <v>172</v>
       </c>
       <c r="F2" t="s">
-        <v>211</v>
+        <v>173</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="D3">
         <v>2023</v>
       </c>
       <c r="E3" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="F3" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2139,410 +2149,410 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.5">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:10" ht="17">
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="17">
+      <c r="A2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="5">
+        <v>30</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2023</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="5">
+        <v>2025</v>
+      </c>
+      <c r="I2" s="5">
+        <v>12</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="6" t="s">
+    </row>
+    <row r="3" spans="1:10" ht="17">
+      <c r="A3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5">
+        <v>6</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G3" s="5">
+        <v>6</v>
+      </c>
+      <c r="H3" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I3" s="5">
+        <v>6</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="17">
+      <c r="A4" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G4" s="5">
+        <v>7</v>
+      </c>
+      <c r="H4" s="5">
+        <v>2022</v>
+      </c>
+      <c r="I4" s="5">
+        <v>6</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="17">
+      <c r="A5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5">
+        <v>8</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G5" s="5">
+        <v>4</v>
+      </c>
+      <c r="H5" s="5">
+        <v>2022</v>
+      </c>
+      <c r="I5" s="5">
+        <v>12</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="17">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="5">
+        <v>2016</v>
+      </c>
+      <c r="G6" s="5">
+        <v>9</v>
+      </c>
+      <c r="H6" s="5">
+        <v>2017</v>
+      </c>
+      <c r="I6" s="5">
+        <v>9</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="17">
+      <c r="A7" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2016</v>
+      </c>
+      <c r="G7" s="5">
+        <v>8</v>
+      </c>
+      <c r="H7" s="5">
+        <v>2016</v>
+      </c>
+      <c r="I7" s="5">
+        <v>12</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="17">
+      <c r="A8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2018</v>
+      </c>
+      <c r="G8" s="5">
+        <v>1</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2021</v>
+      </c>
+      <c r="I8" s="5">
+        <v>12</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="17">
+      <c r="A9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G9" s="5">
+        <v>1</v>
+      </c>
+      <c r="H9" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I9" s="5">
+        <v>12</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="17">
+      <c r="A10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="5">
+        <v>2021</v>
+      </c>
+      <c r="G10" s="5">
+        <v>4</v>
+      </c>
+      <c r="H10" s="5">
+        <v>2023</v>
+      </c>
+      <c r="I10" s="5">
+        <v>12</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="17">
+      <c r="A11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="5">
+        <v>2018</v>
+      </c>
+      <c r="G11" s="5">
+        <v>8</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2020</v>
+      </c>
+      <c r="I11" s="5">
+        <v>6</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="17">
+      <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="C12" s="5"/>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="5">
+        <v>2020</v>
+      </c>
+      <c r="G12" s="5">
+        <v>8</v>
+      </c>
+      <c r="H12" s="5">
+        <v>2020</v>
+      </c>
+      <c r="I12" s="5">
+        <v>12</v>
+      </c>
+      <c r="J12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5">
-      <c r="A2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C2" s="6">
-        <v>30</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="6">
-        <v>2023</v>
-      </c>
-      <c r="G2" s="6">
-        <v>1</v>
-      </c>
-      <c r="H2" s="6">
-        <v>2025</v>
-      </c>
-      <c r="I2" s="6">
+    </row>
+    <row r="13" spans="1:10" ht="17">
+      <c r="A13" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="5">
+        <v>15</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="16.5">
-      <c r="A3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="6">
-        <v>6</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="6">
-        <v>2020</v>
-      </c>
-      <c r="G3" s="6">
-        <v>6</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2023</v>
-      </c>
-      <c r="I3" s="6">
-        <v>6</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5">
-      <c r="A4" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="6">
-        <v>3</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="6">
-        <v>2021</v>
-      </c>
-      <c r="G4" s="6">
-        <v>7</v>
-      </c>
-      <c r="H4" s="6">
+      <c r="E13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="5">
         <v>2022</v>
       </c>
-      <c r="I4" s="6">
-        <v>6</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="16.5">
-      <c r="A5" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="6">
-        <v>8</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="6">
-        <v>2020</v>
-      </c>
-      <c r="G5" s="6">
-        <v>4</v>
-      </c>
-      <c r="H5" s="6">
+      <c r="G13" s="5">
+        <v>10</v>
+      </c>
+      <c r="H13" s="5">
         <v>2022</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I13" s="5">
         <v>12</v>
       </c>
-      <c r="J5" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="16.5">
-      <c r="A6" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="6">
-        <v>5</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F6" s="6">
-        <v>2016</v>
-      </c>
-      <c r="G6" s="6">
-        <v>9</v>
-      </c>
-      <c r="H6" s="6">
-        <v>2017</v>
-      </c>
-      <c r="I6" s="6">
-        <v>9</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="16.5">
-      <c r="A7" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="6">
-        <v>2016</v>
-      </c>
-      <c r="G7" s="6">
-        <v>8</v>
-      </c>
-      <c r="H7" s="6">
-        <v>2016</v>
-      </c>
-      <c r="I7" s="6">
-        <v>12</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="16.5">
-      <c r="A8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F8" s="6">
-        <v>2018</v>
-      </c>
-      <c r="G8" s="6">
-        <v>1</v>
-      </c>
-      <c r="H8" s="6">
-        <v>2021</v>
-      </c>
-      <c r="I8" s="6">
-        <v>12</v>
-      </c>
-      <c r="J8" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="16.5">
-      <c r="A9" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="6">
-        <v>2020</v>
-      </c>
-      <c r="G9" s="6">
-        <v>1</v>
-      </c>
-      <c r="H9" s="6">
-        <v>2023</v>
-      </c>
-      <c r="I9" s="6">
-        <v>12</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="16.5">
-      <c r="A10" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="6">
-        <v>2021</v>
-      </c>
-      <c r="G10" s="6">
-        <v>4</v>
-      </c>
-      <c r="H10" s="6">
-        <v>2023</v>
-      </c>
-      <c r="I10" s="6">
-        <v>12</v>
-      </c>
-      <c r="J10" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="16.5">
-      <c r="A11" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="6">
-        <v>2018</v>
-      </c>
-      <c r="G11" s="6">
-        <v>8</v>
-      </c>
-      <c r="H11" s="6">
-        <v>2020</v>
-      </c>
-      <c r="I11" s="6">
-        <v>6</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="16.5">
-      <c r="A12" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="6">
-        <v>2020</v>
-      </c>
-      <c r="G12" s="6">
-        <v>8</v>
-      </c>
-      <c r="H12" s="6">
-        <v>2020</v>
-      </c>
-      <c r="I12" s="6">
-        <v>12</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16.5">
-      <c r="A13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="6">
-        <v>15</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F13" s="6">
-        <v>2022</v>
-      </c>
-      <c r="G13" s="6">
-        <v>10</v>
-      </c>
-      <c r="H13" s="6">
-        <v>2022</v>
-      </c>
-      <c r="I13" s="6">
-        <v>12</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>66</v>
+      <c r="J13" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -2559,46 +2569,46 @@
       <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
         <v>62</v>
-      </c>
-      <c r="B1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>86</v>
-      </c>
-      <c r="D1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E1" t="s">
-        <v>90</v>
-      </c>
-      <c r="F1" t="s">
-        <v>91</v>
-      </c>
-      <c r="G1" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>188</v>
+        <v>150</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -2615,16 +2625,16 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B3" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
       <c r="E3">
         <v>2</v>
@@ -2641,16 +2651,16 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="C4" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D4" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -2667,16 +2677,16 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>58</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>67</v>
       </c>
       <c r="C5" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="D5" t="s">
-        <v>99</v>
+        <v>68</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -2693,16 +2703,16 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D6" t="s">
-        <v>111</v>
+        <v>80</v>
       </c>
       <c r="E6">
         <v>2</v>
@@ -2717,15 +2727,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5">
+    <row r="7" spans="1:8" ht="17">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B7" t="s">
-        <v>104</v>
+        <v>73</v>
       </c>
       <c r="D7" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -2740,12 +2750,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="16.5">
+    <row r="8" spans="1:8" ht="17">
       <c r="A8" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -2762,10 +2772,10 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2782,10 +2792,10 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>71</v>
       </c>
       <c r="E10">
         <v>1</v>
@@ -2797,12 +2807,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="16.5">
+    <row r="11" spans="1:8" ht="17">
       <c r="A11" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
-        <v>103</v>
+        <v>72</v>
       </c>
       <c r="E11">
         <v>1</v>
@@ -2816,16 +2826,16 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>108</v>
+        <v>77</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>75</v>
       </c>
       <c r="C12" t="s">
-        <v>96</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="E12">
         <v>7</v>
@@ -2842,16 +2852,16 @@
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>107</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
-        <v>189</v>
+        <v>151</v>
       </c>
       <c r="D13" t="s">
-        <v>193</v>
+        <v>155</v>
       </c>
       <c r="E13">
         <v>12</v>
@@ -2868,13 +2878,13 @@
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B14" t="s">
-        <v>194</v>
+        <v>156</v>
       </c>
       <c r="D14" t="s">
-        <v>195</v>
+        <v>157</v>
       </c>
       <c r="E14">
         <v>6</v>
@@ -2891,10 +2901,10 @@
     </row>
     <row r="15" spans="1:8">
       <c r="A15" t="s">
-        <v>110</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>113</v>
+        <v>82</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -2923,20 +2933,20 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="35" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="C1" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2944,7 +2954,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="C2">
         <v>2023</v>
@@ -2955,7 +2965,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="C3">
         <v>2023</v>
@@ -2966,7 +2976,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>186</v>
+        <v>148</v>
       </c>
       <c r="C4">
         <v>2018</v>
@@ -2977,7 +2987,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>187</v>
+        <v>149</v>
       </c>
       <c r="C5">
         <v>2018</v>
@@ -2988,7 +2998,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="C6">
         <v>2024</v>
@@ -2999,7 +3009,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
       <c r="C7">
         <v>2024</v>
@@ -3019,43 +3029,43 @@
       <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>69</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="E1" t="s">
-        <v>75</v>
+        <v>44</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="G1" t="s">
-        <v>70</v>
+        <v>39</v>
       </c>
       <c r="H1" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="I1" t="s">
-        <v>83</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C2">
         <v>40</v>
@@ -3073,15 +3083,15 @@
         <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C3">
         <v>40</v>
@@ -3099,15 +3109,15 @@
         <v>51</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C4">
         <v>40</v>
@@ -3125,15 +3135,15 @@
         <v>28</v>
       </c>
       <c r="H4" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B5" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>32</v>
@@ -3151,15 +3161,15 @@
         <v>34</v>
       </c>
       <c r="H5" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C6">
         <v>16</v>
@@ -3177,15 +3187,15 @@
         <v>23</v>
       </c>
       <c r="H6" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>79</v>
+        <v>48</v>
       </c>
       <c r="B7" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C7">
         <v>32</v>
@@ -3203,15 +3213,15 @@
         <v>8</v>
       </c>
       <c r="H7" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>51</v>
       </c>
       <c r="C8">
         <v>24</v>
@@ -3230,18 +3240,18 @@
         <v>506</v>
       </c>
       <c r="H8" t="s">
-        <v>84</v>
+        <v>53</v>
       </c>
       <c r="I8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="17">
+      <c r="A9" s="2" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="18.75">
-      <c r="A9" s="2" t="s">
-        <v>116</v>
-      </c>
       <c r="B9" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>32</v>
@@ -3259,15 +3269,15 @@
         <v>26</v>
       </c>
       <c r="H9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" ht="16.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="17">
       <c r="A10" s="3" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>32</v>
@@ -3285,15 +3295,15 @@
         <v>36</v>
       </c>
       <c r="H10" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="16.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="17">
       <c r="A11" s="3" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C11">
         <v>32</v>
@@ -3311,15 +3321,15 @@
         <v>71</v>
       </c>
       <c r="H11" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="18.75">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="17">
       <c r="A12" s="2" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -3337,18 +3347,18 @@
         <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="I12" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="18.75">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="17">
       <c r="A13" s="2" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="C13">
         <v>8</v>
@@ -3366,18 +3376,18 @@
         <v>40</v>
       </c>
       <c r="H13" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="I13" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="18.75">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="17">
       <c r="A14" s="2" t="s">
-        <v>116</v>
+        <v>85</v>
       </c>
       <c r="B14" t="s">
-        <v>81</v>
+        <v>50</v>
       </c>
       <c r="C14">
         <v>32</v>
@@ -3395,15 +3405,15 @@
         <v>26</v>
       </c>
       <c r="H14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="16.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="17">
       <c r="A15" s="3" t="s">
-        <v>117</v>
+        <v>86</v>
       </c>
       <c r="B15" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="C15">
         <v>32</v>
@@ -3421,15 +3431,15 @@
         <v>78</v>
       </c>
       <c r="H15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="16.5">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="17">
       <c r="A16" s="3" t="s">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>119</v>
+        <v>88</v>
       </c>
       <c r="C16">
         <v>32</v>
@@ -3447,15 +3457,15 @@
         <v>56</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="18.75">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17">
       <c r="A17" s="2" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
       <c r="C17">
         <v>8</v>
@@ -3473,10 +3483,10 @@
         <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
+        <v>46</v>
       </c>
       <c r="I17" t="s">
-        <v>163</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3493,20 +3503,20 @@
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -3517,10 +3527,10 @@
         <v>2020</v>
       </c>
       <c r="C2" t="s">
-        <v>133</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>134</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3531,10 +3541,10 @@
         <v>2020</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
+        <v>104</v>
       </c>
       <c r="D3" t="s">
-        <v>136</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3545,10 +3555,10 @@
         <v>2020</v>
       </c>
       <c r="C4" t="s">
-        <v>137</v>
+        <v>106</v>
       </c>
       <c r="D4" t="s">
-        <v>138</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3559,10 +3569,10 @@
         <v>2020</v>
       </c>
       <c r="C5" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>140</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -3573,10 +3583,10 @@
         <v>2020</v>
       </c>
       <c r="C6" t="s">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="D6" t="s">
-        <v>142</v>
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -3587,10 +3597,10 @@
         <v>2021</v>
       </c>
       <c r="C7" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="D7" t="s">
-        <v>130</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -3601,10 +3611,10 @@
         <v>2021</v>
       </c>
       <c r="C8" t="s">
-        <v>131</v>
+        <v>100</v>
       </c>
       <c r="D8" t="s">
-        <v>132</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -3615,10 +3625,10 @@
         <v>2022</v>
       </c>
       <c r="C9" t="s">
-        <v>125</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>126</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -3629,10 +3639,10 @@
         <v>2022</v>
       </c>
       <c r="C10" t="s">
-        <v>127</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>97</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -3643,10 +3653,10 @@
         <v>2023</v>
       </c>
       <c r="C11" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -3657,10 +3667,10 @@
         <v>2023</v>
       </c>
       <c r="C12" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>123</v>
+        <v>92</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -3671,10 +3681,10 @@
         <v>2023</v>
       </c>
       <c r="C13" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
       <c r="D13" t="s">
-        <v>124</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -3685,10 +3695,10 @@
         <v>2024</v>
       </c>
       <c r="C14" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="D14" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -3699,10 +3709,10 @@
         <v>2024</v>
       </c>
       <c r="C15" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="D15" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -3719,120 +3729,120 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="3" max="3" width="47.875" customWidth="1"/>
+    <col min="3" max="3" width="47.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="C1" t="s">
-        <v>144</v>
+        <v>113</v>
       </c>
       <c r="D1" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="17.25">
-      <c r="A2" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18">
+      <c r="A2" s="7">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="D2" s="8">
+      <c r="B2" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" s="7">
         <v>2021</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25">
-      <c r="A3" s="8">
+    <row r="3" spans="1:4" ht="18">
+      <c r="A3" s="7">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="D3" s="8">
+      <c r="B3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="D3" s="7">
         <v>2022</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25">
-      <c r="A4" s="8">
+    <row r="4" spans="1:4" ht="18">
+      <c r="A4" s="7">
         <v>3</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="D4" s="8">
+      <c r="B4" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="D4" s="7">
         <v>2023</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25">
-      <c r="A5" s="8">
+    <row r="5" spans="1:4" ht="18">
+      <c r="A5" s="7">
         <v>4</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>220</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="D5" s="8">
+      <c r="B5" s="7" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="D5" s="7">
         <v>2023</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:4" ht="18">
+      <c r="A6" s="7">
         <v>5</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="B6" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="D6" s="7">
         <v>2024</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25">
-      <c r="A7" s="8">
+    <row r="7" spans="1:4" ht="18">
+      <c r="A7" s="7">
         <v>6</v>
       </c>
-      <c r="B7" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>226</v>
-      </c>
-      <c r="D7" s="8">
+      <c r="B7" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>188</v>
+      </c>
+      <c r="D7" s="7">
         <v>2024</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="17.25">
-      <c r="A8" s="8">
+    <row r="8" spans="1:4" ht="18">
+      <c r="A8" s="7">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>221</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>227</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="B8" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="7">
         <v>2024</v>
       </c>
     </row>
@@ -3850,23 +3860,23 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
         <v>91</v>
       </c>
-      <c r="C1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="18.75">
+    </row>
+    <row r="2" spans="1:6" ht="17">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3874,13 +3884,13 @@
         <v>2023</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>146</v>
+        <v>115</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="18.75">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="17">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3888,13 +3898,13 @@
         <v>2023</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>148</v>
+        <v>117</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="18.75">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="17">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3902,13 +3912,13 @@
         <v>2023</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>149</v>
+        <v>118</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="18.75">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="17">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3916,13 +3926,13 @@
         <v>2023</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>151</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="18.75">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="17">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3930,15 +3940,15 @@
         <v>2024</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>196</v>
+        <v>158</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>197</v>
+        <v>159</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="18.75">
+    <row r="7" spans="1:6" ht="17">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3946,15 +3956,15 @@
         <v>2024</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>198</v>
+        <v>160</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
     </row>
-    <row r="8" spans="1:6" ht="18.75">
+    <row r="8" spans="1:6" ht="17">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3962,15 +3972,15 @@
         <v>2024</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>199</v>
+        <v>161</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>200</v>
+        <v>162</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="18.75">
+    <row r="9" spans="1:6" ht="17">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3978,15 +3988,15 @@
         <v>2024</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>201</v>
+        <v>163</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>202</v>
+        <v>164</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
     </row>
-    <row r="10" spans="1:6" ht="18.75">
+    <row r="10" spans="1:6" ht="17">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3994,10 +4004,10 @@
         <v>2024</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>212</v>
+        <v>174</v>
       </c>
       <c r="D10" t="s">
-        <v>213</v>
+        <v>175</v>
       </c>
     </row>
   </sheetData>

</xml_diff>